<commit_message>
Actualizacion Cronograma Angel Chacon
</commit_message>
<xml_diff>
--- a/P3GA2/Cronograma Practica PROGRA.xlsx
+++ b/P3GA2/Cronograma Practica PROGRA.xlsx
@@ -491,36 +491,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -544,15 +514,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -588,13 +549,52 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -869,7 +869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -878,10 +878,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="B1:H67"/>
+  <dimension ref="B1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -896,24 +896,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
@@ -988,7 +988,7 @@
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="20" t="s">
         <v>11</v>
       </c>
@@ -998,7 +998,7 @@
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="14" t="s">
         <v>15</v>
       </c>
@@ -1034,10 +1034,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
+      <c r="B13" s="53"/>
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="25"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="15"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1045,7 +1045,7 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="25"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="17" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="25"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="14" t="s">
         <v>27</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="14" t="s">
         <v>17</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="14" t="s">
         <v>18</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
+      <c r="B20" s="60"/>
       <c r="C20" s="14" t="s">
         <v>19</v>
       </c>
@@ -1146,7 +1146,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="14" t="s">
         <v>20</v>
       </c>
@@ -1188,7 +1188,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="24"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="14" t="s">
         <v>22</v>
       </c>
@@ -1209,7 +1209,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="14" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="26"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="14" t="s">
         <v>24</v>
       </c>
@@ -1272,7 +1272,7 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="14" t="s">
         <v>26</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="14" t="s">
         <v>34</v>
       </c>
@@ -1315,487 +1315,495 @@
     </row>
     <row r="29" spans="2:8" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B29" s="8"/>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="58" t="s">
+      <c r="C30" s="41"/>
+      <c r="D30" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="38" t="s">
+      <c r="E30" s="50"/>
+      <c r="F30" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="41"/>
     </row>
     <row r="31" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="56" t="s">
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="57">
-        <v>0</v>
-      </c>
-      <c r="H31" s="39" t="s">
+      <c r="G31" s="44">
+        <v>0</v>
+      </c>
+      <c r="H31" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="53" t="s">
+      <c r="F32" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="33">
-        <v>0</v>
-      </c>
-      <c r="H32" s="39" t="s">
+      <c r="G32" s="23">
+        <v>0</v>
+      </c>
+      <c r="H32" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B33" s="8"/>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="53" t="s">
+      <c r="F33" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="33">
+      <c r="G33" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B34" s="8"/>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="53" t="s">
+      <c r="F34" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="33">
+      <c r="G34" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B35" s="8"/>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="27" t="s">
         <v>42</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="33">
+      <c r="F35" s="40"/>
+      <c r="G35" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
-      <c r="C36" s="52" t="s">
-        <v>43</v>
-      </c>
+      <c r="C36" s="27"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="33">
-        <v>0</v>
-      </c>
+      <c r="F36" s="40"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B37" s="8"/>
-      <c r="C37" s="35" t="s">
-        <v>27</v>
+      <c r="C37" s="39" t="s">
+        <v>43</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
-      <c r="F37" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" s="33">
-        <v>0</v>
-      </c>
-      <c r="H37" s="41" t="s">
-        <v>50</v>
+      <c r="F37" s="40"/>
+      <c r="G37" s="23">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B38" s="8"/>
-      <c r="C38" s="35" t="s">
-        <v>44</v>
+      <c r="C38" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
-      <c r="F38" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="33">
-        <v>0</v>
-      </c>
-      <c r="H38" s="41" t="s">
+      <c r="F38" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" s="23">
+        <v>0</v>
+      </c>
+      <c r="H38" s="31" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
-      <c r="C39" s="35"/>
+      <c r="C39" s="25" t="s">
+        <v>44</v>
+      </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="33"/>
+      <c r="F39" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="23">
+        <v>0</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B40" s="8"/>
-      <c r="C40" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="39"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B41" s="8"/>
-      <c r="C41" s="14" t="s">
-        <v>18</v>
+      <c r="C41" s="45" t="s">
+        <v>51</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="33">
-        <v>0</v>
-      </c>
-      <c r="H41" s="39" t="s">
-        <v>46</v>
-      </c>
+      <c r="F41" s="40"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B42" s="8"/>
       <c r="C42" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="53" t="s">
+      <c r="F42" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="33">
-        <v>0</v>
-      </c>
-      <c r="H42" s="39" t="s">
+      <c r="G42" s="23">
+        <v>0</v>
+      </c>
+      <c r="H42" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B43" s="8"/>
       <c r="C43" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="53" t="s">
+      <c r="F43" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="33">
-        <v>0</v>
-      </c>
-      <c r="H43" s="39" t="s">
+      <c r="G43" s="23">
+        <v>0</v>
+      </c>
+      <c r="H43" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B44" s="8"/>
       <c r="C44" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="G44" s="33">
-        <v>0</v>
-      </c>
-      <c r="H44" s="39" t="s">
+      <c r="F44" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="23">
+        <v>0</v>
+      </c>
+      <c r="H44" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B45" s="8"/>
       <c r="C45" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="53" t="s">
+      <c r="F45" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="33">
-        <v>0</v>
-      </c>
-      <c r="H45" s="39" t="s">
+      <c r="G45" s="23">
+        <v>0</v>
+      </c>
+      <c r="H45" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B46" s="8"/>
       <c r="C46" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
-      <c r="F46" s="53" t="s">
+      <c r="F46" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G46" s="33">
-        <v>0</v>
-      </c>
-      <c r="H46" s="39" t="s">
+      <c r="G46" s="23">
+        <v>0</v>
+      </c>
+      <c r="H46" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B47" s="8"/>
       <c r="C47" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="G47" s="33">
-        <v>0</v>
-      </c>
-      <c r="H47" s="39" t="s">
+      <c r="F47" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" s="23">
+        <v>0</v>
+      </c>
+      <c r="H47" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B48" s="8"/>
       <c r="C48" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="53" t="s">
+      <c r="F48" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G48" s="33">
-        <v>0</v>
-      </c>
-      <c r="H48" s="39" t="s">
+      <c r="G48" s="23">
+        <v>0</v>
+      </c>
+      <c r="H48" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B49" s="8"/>
       <c r="C49" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
-      <c r="F49" s="53" t="s">
+      <c r="F49" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G49" s="33">
-        <v>0</v>
-      </c>
-      <c r="H49" s="39" t="s">
+      <c r="G49" s="23">
+        <v>0</v>
+      </c>
+      <c r="H49" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B50" s="8"/>
       <c r="C50" s="14" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
-      <c r="F50" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="G50" s="33">
-        <v>0</v>
-      </c>
-      <c r="H50" s="39" t="s">
+      <c r="F50" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G50" s="23">
+        <v>0</v>
+      </c>
+      <c r="H50" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B51" s="8"/>
-      <c r="C51" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="53" t="s">
+      <c r="C51" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="33">
-        <v>0</v>
-      </c>
-      <c r="H51" s="39" t="s">
+      <c r="G51" s="23">
+        <v>0</v>
+      </c>
+      <c r="H51" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B52" s="8"/>
-      <c r="C52" s="35" t="s">
-        <v>44</v>
+      <c r="C52" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
-      <c r="F52" s="53" t="s">
+      <c r="F52" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="33">
-        <v>0</v>
-      </c>
-      <c r="H52" s="39" t="s">
+      <c r="G52" s="23">
+        <v>0</v>
+      </c>
+      <c r="H52" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B53" s="8"/>
-      <c r="C53" s="35"/>
+      <c r="C53" s="25" t="s">
+        <v>44</v>
+      </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="39"/>
+      <c r="F53" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="23">
+        <v>0</v>
+      </c>
+      <c r="H53" s="29" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="54" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B54" s="8"/>
-      <c r="C54" s="38" t="s">
-        <v>45</v>
-      </c>
+      <c r="C54" s="25"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
-      <c r="F54" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="G54" s="33">
-        <v>0</v>
-      </c>
+      <c r="F54" s="40"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="29"/>
     </row>
     <row r="55" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B55" s="8"/>
-      <c r="C55" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="12">
-        <v>43964</v>
-      </c>
-      <c r="E55" s="12">
-        <v>43965</v>
-      </c>
-      <c r="F55" s="53" t="s">
+      <c r="C55" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G55" s="33">
+      <c r="G55" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B56" s="8"/>
-      <c r="C56" s="22" t="s">
-        <v>33</v>
+      <c r="C56" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="D56" s="12">
         <v>43964</v>
       </c>
       <c r="E56" s="12">
+        <v>43965</v>
+      </c>
+      <c r="F56" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B57" s="8"/>
+      <c r="C57" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="12">
+        <v>43964</v>
+      </c>
+      <c r="E57" s="12">
         <v>43972</v>
       </c>
-      <c r="F56" s="53" t="s">
+      <c r="F57" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G56" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B57" s="40"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="49"/>
+      <c r="G57" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B58" s="40"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="49"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
     </row>
     <row r="59" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B59" s="50"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="37" t="s">
+      <c r="B59" s="30"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="36"/>
+    </row>
+    <row r="60" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B60" s="37"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G59" s="7">
-        <f>AVERAGE(G5:G56)</f>
+      <c r="G60" s="7">
+        <f>AVERAGE(G5:G57)</f>
         <v>0.39342105263157895</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B60" s="40"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="49"/>
-    </row>
     <row r="61" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B61" s="50"/>
-      <c r="C61" s="45"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="49"/>
-    </row>
-    <row r="62" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B62" s="40"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="36"/>
+    </row>
+    <row r="62" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B62" s="37"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="36"/>
     </row>
     <row r="63" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B63" s="40"/>
+      <c r="B63" s="30"/>
     </row>
     <row r="64" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B64" s="40"/>
+      <c r="B64" s="30"/>
     </row>
     <row r="65" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B65" s="40"/>
-    </row>
-    <row r="66" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B65" s="30"/>
+    </row>
+    <row r="66" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B66" s="30"/>
+    </row>
     <row r="67" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C29:G29"/>

</xml_diff>